<commit_message>
Atualização planilha - planning poker
</commit_message>
<xml_diff>
--- a/Gerenciamento de Projeto/epcafe - Planejamento e Controle do Projeto.xlsx
+++ b/Gerenciamento de Projeto/epcafe - Planejamento e Controle do Projeto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe Nora Godinho\epcafe-grupo5\Gerenciamento de Projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Notebook\epcafe-grupo5\Gerenciamento de Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -128,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -138,25 +138,25 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">Resultado do Planning Poker, convertido para horas.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">O identificador da trefa auxilia na criação e uso dos "Post-it" dos quadros Kanban ou Scrum.
 </t>
         </r>
       </text>
     </comment>
     <comment ref="G3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">O identificador da trefa auxilia na criação e uso dos "Post-it" dos quadros Kanban ou Scrum.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -184,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0">
+    <comment ref="I4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -206,30 +206,6 @@
           <t xml:space="preserve">
 V = Valor: Quanto de valor a história de usuário representa para o usuário final?
 </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Pontue de 0 a 10.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">R = Risco: Qual é o risco desta história não ser entregue? </t>
         </r>
       </text>
     </comment>
@@ -243,7 +219,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Somente 10 quando existe Dependência, do contrário 0.
+          <t xml:space="preserve">Pontue de 0 a 10.
 </t>
         </r>
         <r>
@@ -253,8 +229,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>D = Dependência: A história que será pontuada, irá gerar insumos para “outras” histórias no Backlog?
-Ex: Temos duas histórias no Backlog, A e B. A história A não consegue ser entregue pois necessita que a história B seja entregue antes. Diante disso a história B receberá a pontuação “10” no método VRDC pois ela precisa ser completada o mais rápido possível para que a história A também seja entregue.</t>
+          <t xml:space="preserve">R = Risco: Qual é o risco desta história não ser entregue? </t>
         </r>
       </text>
     </comment>
@@ -268,7 +243,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Pontue de 0 a 10.</t>
+          <t xml:space="preserve">Somente 10 quando existe Dependência, do contrário 0.
+</t>
         </r>
         <r>
           <rPr>
@@ -277,12 +253,36 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
-C = Complexidade Técnica: Qual a complexidade técnica (tecnologia) da história?</t>
+          <t>D = Dependência: A história que será pontuada, irá gerar insumos para “outras” histórias no Backlog?
+Ex: Temos duas histórias no Backlog, A e B. A história A não consegue ser entregue pois necessita que a história B seja entregue antes. Diante disso a história B receberá a pontuação “10” no método VRDC pois ela precisa ser completada o mais rápido possível para que a história A também seja entregue.</t>
         </r>
       </text>
     </comment>
     <comment ref="L4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pontue de 0 a 10.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+C = Complexidade Técnica: Qual a complexidade técnica (tecnologia) da história?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1935,7 +1935,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="261">
   <si>
     <t>Iniciação</t>
   </si>
@@ -2589,12 +2589,6 @@
     <t>Ajuste base histórica (margem de erro da estimativa)</t>
   </si>
   <si>
-    <t>UC01</t>
-  </si>
-  <si>
-    <t>Modelar UC1</t>
-  </si>
-  <si>
     <t>Definir escopo</t>
   </si>
   <si>
@@ -2610,9 +2604,6 @@
     <t>Planejar o Sprint</t>
   </si>
   <si>
-    <t>Especificar UC01-Manter Clubes</t>
-  </si>
-  <si>
     <t>Aplicar Checlist da fase</t>
   </si>
   <si>
@@ -2637,21 +2628,6 @@
     <t>Implementar e testar a arquitetura</t>
   </si>
   <si>
-    <t>Implementar e testar unitariamente U02</t>
-  </si>
-  <si>
-    <t>Executar Testes UC02</t>
-  </si>
-  <si>
-    <t>Projetar Testes UC02</t>
-  </si>
-  <si>
-    <t>Especificar UC02-Manter Atleta</t>
-  </si>
-  <si>
-    <t>Modelar UC2</t>
-  </si>
-  <si>
     <t>Projetar Testes de Sistema</t>
   </si>
   <si>
@@ -2674,9 +2650,6 @@
   </si>
   <si>
     <t>Casos de Uso ou Histórias de Usuário</t>
-  </si>
-  <si>
-    <t>UC03</t>
   </si>
   <si>
     <t>Estimativa</t>
@@ -2707,42 +2680,15 @@
 Desse modo, basta inserir os casos de uso/histórias específicos do projeto.</t>
   </si>
   <si>
-    <t>UC02</t>
-  </si>
-  <si>
     <t>Estudar tecnologias</t>
   </si>
   <si>
     <t>Preparar Ambiente de Desenvolvimento</t>
   </si>
   <si>
-    <t>Especificar UC01-Manter Clubes (escolhido para testar a arquitetura)</t>
-  </si>
-  <si>
-    <t>Modelar UC1 e Arquitetura</t>
-  </si>
-  <si>
     <t>Implementar e testar unitariamente U01</t>
   </si>
   <si>
-    <t>Especificar UC03-Manter Categorias</t>
-  </si>
-  <si>
-    <t>Modelar UC3</t>
-  </si>
-  <si>
-    <t>Implementar e testar unitariamente U03</t>
-  </si>
-  <si>
-    <t>Projetar Testes UC03</t>
-  </si>
-  <si>
-    <t>Executar Testes UC03</t>
-  </si>
-  <si>
-    <t>Especificar UC???</t>
-  </si>
-  <si>
     <t>Jornada de trabalho semanal por desenvolvedor</t>
   </si>
   <si>
@@ -2818,40 +2764,46 @@
     <t>Guilherme Quirino Pessoa De Araújo Cruz</t>
   </si>
   <si>
-    <t>lucas.freitas@aluno.ifsp.edu.br</t>
-  </si>
-  <si>
-    <t>guilherme.cruz@aluno.ifsp.edu.br</t>
-  </si>
-  <si>
     <t>vinicius.valim@aluno.ifsp.edu.br</t>
   </si>
   <si>
-    <t>Sim</t>
-  </si>
-  <si>
-    <t>RM#001 - Criação do Repositório GitHub</t>
-  </si>
-  <si>
-    <t>RM#002 - Elaboração do Modelo de Caso de Uso</t>
-  </si>
-  <si>
-    <t>RM#003 - Desenvolvimento do documento "Visão"</t>
-  </si>
-  <si>
-    <t>RM#004 - Primeira versão da planilha de Planejamento e Controle</t>
-  </si>
-  <si>
     <t>ES1 - èpCafé</t>
   </si>
   <si>
-    <t>Visão, modelo de caso de uso plainilha de controle</t>
-  </si>
-  <si>
     <t>Em execução</t>
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>UC01 - Gerar relatorio de usuarios logados por unidade</t>
+  </si>
+  <si>
+    <t>Sistema de login ser incompativel com a funcionalidade de controle de sessão</t>
+  </si>
+  <si>
+    <t>1. Trabalho sincrono com o grupo de desenvolvimento responsavel</t>
+  </si>
+  <si>
+    <t>RM#001 -</t>
+  </si>
+  <si>
+    <t>Modelagem final UC1</t>
+  </si>
+  <si>
+    <t>História do Usuário UC01</t>
+  </si>
+  <si>
+    <t>Especificar UC01</t>
+  </si>
+  <si>
+    <t>guilherme.quirino@aluno.ifsp.edu.br</t>
+  </si>
+  <si>
+    <t>t.freitas@aluno.ifsp.edu.br</t>
+  </si>
+  <si>
+    <t>Modelagem inicial UC01 e Arquitetura</t>
   </si>
 </sst>
 </file>
@@ -3557,7 +3509,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="208">
+  <cellXfs count="210">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3986,6 +3938,13 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4068,6 +4027,21 @@
     <xf numFmtId="0" fontId="26" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4089,9 +4063,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4103,18 +4074,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4171,22 +4130,7 @@
     <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
     <cellStyle name="Vírgula" xfId="3" builtinId="3"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="54"/>
-      </font>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <b/>
@@ -4222,6 +4166,36 @@
           <bgColor indexed="42"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="54"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="54"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -4341,7 +4315,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4724,7 +4697,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5341,15 +5313,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>525463</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6525,7 +6497,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6536,18 +6508,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="152" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="150"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
     </row>
     <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="151" t="s">
-        <v>273</v>
-      </c>
-      <c r="B2" s="151"/>
-      <c r="C2" s="151"/>
+      <c r="A2" s="153" t="s">
+        <v>248</v>
+      </c>
+      <c r="B2" s="153"/>
+      <c r="C2" s="153"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -6565,21 +6537,21 @@
         <v>44</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -6587,10 +6559,10 @@
         <v>45</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -6598,10 +6570,10 @@
         <v>45</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -6620,10 +6592,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6631,109 +6603,114 @@
     <col min="1" max="1" width="11" style="51" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="22" customWidth="1"/>
     <col min="3" max="3" width="69" style="22" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="124" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.7109375" style="22" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" style="22" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="22"/>
-    <col min="10" max="10" width="11.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="22" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="22"/>
+    <col min="4" max="4" width="10" style="22" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="124" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="22"/>
+    <col min="11" max="11" width="11.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="22" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="162" t="s">
+    <row r="1" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="164" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="F1" s="155" t="s">
-        <v>220</v>
-      </c>
-      <c r="G1" s="156"/>
-      <c r="H1" s="156"/>
-      <c r="I1" s="156"/>
-      <c r="J1" s="156"/>
-      <c r="K1" s="156"/>
-      <c r="L1" s="156"/>
-    </row>
-    <row r="2" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="157" t="s">
-        <v>227</v>
-      </c>
-      <c r="B2" s="158"/>
-      <c r="C2" s="158"/>
-      <c r="D2" s="158"/>
-      <c r="F2" s="159" t="s">
-        <v>252</v>
-      </c>
-      <c r="G2" s="160"/>
-      <c r="H2" s="160"/>
-      <c r="I2" s="160"/>
-      <c r="J2" s="160"/>
-      <c r="K2" s="160"/>
-      <c r="L2" s="160"/>
-    </row>
-    <row r="3" spans="1:12" ht="24" x14ac:dyDescent="0.2">
+      <c r="B1" s="165"/>
+      <c r="C1" s="165"/>
+      <c r="D1" s="165"/>
+      <c r="E1" s="165"/>
+      <c r="G1" s="157" t="s">
+        <v>211</v>
+      </c>
+      <c r="H1" s="158"/>
+      <c r="I1" s="158"/>
+      <c r="J1" s="158"/>
+      <c r="K1" s="158"/>
+      <c r="L1" s="158"/>
+      <c r="M1" s="158"/>
+    </row>
+    <row r="2" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="159" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" s="160"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="160"/>
+      <c r="G2" s="161" t="s">
+        <v>234</v>
+      </c>
+      <c r="H2" s="162"/>
+      <c r="I2" s="162"/>
+      <c r="J2" s="162"/>
+      <c r="K2" s="162"/>
+      <c r="L2" s="162"/>
+      <c r="M2" s="162"/>
+    </row>
+    <row r="3" spans="1:13" ht="12" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
         <v>135</v>
       </c>
       <c r="B3" s="138" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C3" s="138" t="s">
-        <v>200</v>
-      </c>
-      <c r="D3" s="138" t="s">
-        <v>219</v>
-      </c>
-      <c r="F3" s="138" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="151"/>
+      <c r="E3" s="138" t="s">
+        <v>210</v>
+      </c>
+      <c r="G3" s="138" t="s">
         <v>135</v>
       </c>
-      <c r="G3" s="139" t="s">
+      <c r="H3" s="139" t="s">
+        <v>209</v>
+      </c>
+      <c r="I3" s="163" t="s">
+        <v>211</v>
+      </c>
+      <c r="J3" s="163"/>
+      <c r="K3" s="163"/>
+      <c r="L3" s="163"/>
+      <c r="M3" s="163"/>
+    </row>
+    <row r="4" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+      <c r="A4" s="154" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="155"/>
+      <c r="C4" s="156"/>
+      <c r="D4" s="150"/>
+      <c r="E4" s="131" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="129" t="s">
         <v>217</v>
       </c>
-      <c r="H3" s="161" t="s">
-        <v>220</v>
-      </c>
-      <c r="I3" s="161"/>
-      <c r="J3" s="161"/>
-      <c r="K3" s="161"/>
-      <c r="L3" s="161"/>
-    </row>
-    <row r="4" spans="1:12" ht="24" x14ac:dyDescent="0.2">
-      <c r="A4" s="152" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="153"/>
-      <c r="C4" s="154"/>
-      <c r="D4" s="131" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="129" t="s">
-        <v>226</v>
-      </c>
-      <c r="G4" s="129" t="s">
-        <v>225</v>
-      </c>
-      <c r="H4" s="131" t="s">
-        <v>221</v>
+      <c r="H4" s="129" t="s">
+        <v>216</v>
       </c>
       <c r="I4" s="131" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="J4" s="131" t="s">
-        <v>223</v>
-      </c>
-      <c r="K4" s="136" t="s">
-        <v>224</v>
-      </c>
-      <c r="L4" s="131" t="s">
+        <v>213</v>
+      </c>
+      <c r="K4" s="131" t="s">
+        <v>214</v>
+      </c>
+      <c r="L4" s="136" t="s">
+        <v>215</v>
+      </c>
+      <c r="M4" s="131" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="126">
         <v>1</v>
       </c>
@@ -6741,35 +6718,39 @@
         <v>0</v>
       </c>
       <c r="C5" s="140" t="s">
-        <v>194</v>
-      </c>
-      <c r="D5" s="133">
-        <v>10</v>
-      </c>
-      <c r="F5" s="127">
+        <v>192</v>
+      </c>
+      <c r="D5" s="140">
+        <f>E5*0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="133">
         <v>1</v>
       </c>
-      <c r="G5" s="140" t="s">
-        <v>189</v>
-      </c>
-      <c r="H5" s="130">
-        <v>5</v>
+      <c r="G5" s="127">
+        <v>1</v>
+      </c>
+      <c r="H5" s="140" t="s">
+        <v>251</v>
       </c>
       <c r="I5" s="130">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J5" s="130">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K5" s="130">
-        <v>3</v>
-      </c>
-      <c r="L5" s="132">
-        <f>SUM(H5:K5)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="130">
+        <v>6</v>
+      </c>
+      <c r="M5" s="132">
+        <f>SUM(I5:L5)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="126">
         <v>2</v>
       </c>
@@ -6777,35 +6758,29 @@
         <v>0</v>
       </c>
       <c r="C6" s="140" t="s">
-        <v>192</v>
-      </c>
-      <c r="D6" s="133">
-        <v>10</v>
-      </c>
-      <c r="F6" s="127">
+        <v>190</v>
+      </c>
+      <c r="D6" s="140">
+        <f t="shared" ref="D6:D42" si="0">E6*0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="133">
+        <v>1</v>
+      </c>
+      <c r="G6" s="127">
         <v>2</v>
       </c>
-      <c r="G6" s="140" t="s">
-        <v>228</v>
-      </c>
-      <c r="H6" s="130">
-        <v>5</v>
-      </c>
-      <c r="I6" s="130">
+      <c r="H6" s="140"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="130"/>
+      <c r="K6" s="130"/>
+      <c r="L6" s="130"/>
+      <c r="M6" s="132">
+        <f t="shared" ref="M6:M18" si="1">SUM(I6:L6)</f>
         <v>0</v>
       </c>
-      <c r="J6" s="130">
-        <v>5</v>
-      </c>
-      <c r="K6" s="130">
-        <v>5</v>
-      </c>
-      <c r="L6" s="132">
-        <f t="shared" ref="L6:L19" si="0">SUM(H6:K6)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="126">
         <v>3</v>
       </c>
@@ -6813,35 +6788,29 @@
         <v>0</v>
       </c>
       <c r="C7" s="140" t="s">
-        <v>191</v>
-      </c>
-      <c r="D7" s="133">
-        <v>15</v>
-      </c>
-      <c r="F7" s="127">
+        <v>189</v>
+      </c>
+      <c r="D7" s="140">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E7" s="133">
+        <v>4</v>
+      </c>
+      <c r="G7" s="127">
         <v>3</v>
       </c>
-      <c r="G7" s="140" t="s">
-        <v>218</v>
-      </c>
-      <c r="H7" s="130">
-        <v>3</v>
-      </c>
-      <c r="I7" s="130">
+      <c r="H7" s="140"/>
+      <c r="I7" s="130"/>
+      <c r="J7" s="130"/>
+      <c r="K7" s="130"/>
+      <c r="L7" s="130"/>
+      <c r="M7" s="132">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J7" s="130">
-        <v>0</v>
-      </c>
-      <c r="K7" s="130">
-        <v>3</v>
-      </c>
-      <c r="L7" s="132">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="126">
         <v>4</v>
       </c>
@@ -6849,23 +6818,27 @@
         <v>0</v>
       </c>
       <c r="C8" s="140" t="s">
-        <v>193</v>
-      </c>
-      <c r="D8" s="133">
-        <v>15</v>
-      </c>
-      <c r="F8" s="127"/>
-      <c r="G8" s="140"/>
-      <c r="H8" s="130"/>
+        <v>191</v>
+      </c>
+      <c r="D8" s="140">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E8" s="133">
+        <v>8</v>
+      </c>
+      <c r="G8" s="127"/>
+      <c r="H8" s="140"/>
       <c r="I8" s="130"/>
       <c r="J8" s="130"/>
       <c r="K8" s="130"/>
-      <c r="L8" s="132">
-        <f t="shared" si="0"/>
+      <c r="L8" s="130"/>
+      <c r="M8" s="132">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="126">
         <v>5</v>
       </c>
@@ -6873,23 +6846,27 @@
         <v>0</v>
       </c>
       <c r="C9" s="140" t="s">
-        <v>197</v>
-      </c>
-      <c r="D9" s="133">
-        <v>10</v>
-      </c>
-      <c r="F9" s="128"/>
-      <c r="G9" s="140"/>
-      <c r="H9" s="130"/>
+        <v>195</v>
+      </c>
+      <c r="D9" s="140">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="133">
+        <v>1</v>
+      </c>
+      <c r="G9" s="128"/>
+      <c r="H9" s="140"/>
       <c r="I9" s="130"/>
       <c r="J9" s="130"/>
       <c r="K9" s="130"/>
-      <c r="L9" s="132">
-        <f t="shared" si="0"/>
+      <c r="L9" s="130"/>
+      <c r="M9" s="132">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="126">
         <v>6</v>
       </c>
@@ -6897,44 +6874,52 @@
         <v>0</v>
       </c>
       <c r="C10" s="140" t="s">
-        <v>202</v>
-      </c>
-      <c r="D10" s="133">
+        <v>199</v>
+      </c>
+      <c r="D10" s="140">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10" s="133">
         <v>2</v>
       </c>
-      <c r="F10" s="127"/>
-      <c r="G10" s="140"/>
-      <c r="H10" s="130"/>
+      <c r="G10" s="127"/>
+      <c r="H10" s="140"/>
       <c r="I10" s="130"/>
       <c r="J10" s="130"/>
       <c r="K10" s="130"/>
-      <c r="L10" s="132">
-        <f t="shared" si="0"/>
+      <c r="L10" s="130"/>
+      <c r="M10" s="132">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="152" t="s">
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="154" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="153"/>
-      <c r="C11" s="154"/>
+      <c r="B11" s="155"/>
+      <c r="C11" s="156"/>
       <c r="D11" s="131">
         <f>SUM(D5:D10)</f>
-        <v>62</v>
-      </c>
-      <c r="F11" s="128"/>
-      <c r="G11" s="140"/>
-      <c r="H11" s="130"/>
+        <v>8.5</v>
+      </c>
+      <c r="E11" s="131">
+        <f>SUM(E5:E10)</f>
+        <v>17</v>
+      </c>
+      <c r="G11" s="128"/>
+      <c r="H11" s="140"/>
       <c r="I11" s="130"/>
       <c r="J11" s="130"/>
       <c r="K11" s="130"/>
-      <c r="L11" s="132">
-        <f t="shared" si="0"/>
+      <c r="L11" s="130"/>
+      <c r="M11" s="132">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="126">
         <v>7</v>
       </c>
@@ -6942,21 +6927,27 @@
         <v>1</v>
       </c>
       <c r="C12" s="140" t="s">
-        <v>195</v>
-      </c>
-      <c r="D12" s="133"/>
-      <c r="F12" s="128"/>
-      <c r="G12" s="140"/>
-      <c r="H12" s="130"/>
+        <v>193</v>
+      </c>
+      <c r="D12" s="140">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E12" s="133">
+        <v>4</v>
+      </c>
+      <c r="G12" s="128"/>
+      <c r="H12" s="140"/>
       <c r="I12" s="130"/>
       <c r="J12" s="130"/>
       <c r="K12" s="130"/>
-      <c r="L12" s="132">
-        <f t="shared" si="0"/>
+      <c r="L12" s="130"/>
+      <c r="M12" s="132">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="126">
         <v>8</v>
       </c>
@@ -6964,21 +6955,27 @@
         <v>1</v>
       </c>
       <c r="C13" s="140" t="s">
-        <v>229</v>
-      </c>
-      <c r="D13" s="133"/>
-      <c r="F13" s="128"/>
-      <c r="G13" s="140"/>
-      <c r="H13" s="130"/>
+        <v>219</v>
+      </c>
+      <c r="D13" s="140">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E13" s="133">
+        <v>30</v>
+      </c>
+      <c r="G13" s="128"/>
+      <c r="H13" s="140"/>
       <c r="I13" s="130"/>
       <c r="J13" s="130"/>
       <c r="K13" s="130"/>
-      <c r="L13" s="132">
-        <f t="shared" si="0"/>
+      <c r="L13" s="130"/>
+      <c r="M13" s="132">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="126">
         <v>9</v>
       </c>
@@ -6986,21 +6983,27 @@
         <v>1</v>
       </c>
       <c r="C14" s="125" t="s">
-        <v>230</v>
-      </c>
-      <c r="D14" s="133"/>
-      <c r="F14" s="128"/>
-      <c r="G14" s="140"/>
-      <c r="H14" s="130"/>
+        <v>220</v>
+      </c>
+      <c r="D14" s="140">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="E14" s="133">
+        <v>5</v>
+      </c>
+      <c r="G14" s="128"/>
+      <c r="H14" s="140"/>
       <c r="I14" s="130"/>
       <c r="J14" s="130"/>
       <c r="K14" s="130"/>
-      <c r="L14" s="132">
-        <f t="shared" si="0"/>
+      <c r="L14" s="130"/>
+      <c r="M14" s="132">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="126">
         <v>10</v>
       </c>
@@ -7008,21 +7011,27 @@
         <v>1</v>
       </c>
       <c r="C15" s="141" t="s">
-        <v>231</v>
-      </c>
-      <c r="D15" s="133"/>
-      <c r="F15" s="128"/>
-      <c r="G15" s="140"/>
-      <c r="H15" s="130"/>
+        <v>256</v>
+      </c>
+      <c r="D15" s="140">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="E15" s="133">
+        <v>5</v>
+      </c>
+      <c r="G15" s="128"/>
+      <c r="H15" s="140"/>
       <c r="I15" s="130"/>
       <c r="J15" s="130"/>
       <c r="K15" s="130"/>
-      <c r="L15" s="132">
-        <f t="shared" si="0"/>
+      <c r="L15" s="130"/>
+      <c r="M15" s="132">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="126">
         <v>11</v>
       </c>
@@ -7030,43 +7039,55 @@
         <v>1</v>
       </c>
       <c r="C16" s="142" t="s">
-        <v>232</v>
-      </c>
-      <c r="D16" s="133"/>
-      <c r="F16" s="128"/>
-      <c r="G16" s="140"/>
-      <c r="H16" s="130"/>
+        <v>260</v>
+      </c>
+      <c r="D16" s="140">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E16" s="133">
+        <v>10</v>
+      </c>
+      <c r="G16" s="128"/>
+      <c r="H16" s="140"/>
       <c r="I16" s="130"/>
       <c r="J16" s="130"/>
       <c r="K16" s="130"/>
-      <c r="L16" s="132">
-        <f t="shared" si="0"/>
+      <c r="L16" s="130"/>
+      <c r="M16" s="132">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="126">
         <v>12</v>
       </c>
       <c r="B17" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="142" t="s">
-        <v>233</v>
-      </c>
-      <c r="D17" s="133"/>
-      <c r="F17" s="128"/>
-      <c r="G17" s="140"/>
-      <c r="H17" s="130"/>
+      <c r="C17" s="125" t="s">
+        <v>198</v>
+      </c>
+      <c r="D17" s="140">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E17" s="133">
+        <v>8</v>
+      </c>
+      <c r="G17" s="128"/>
+      <c r="H17" s="140"/>
       <c r="I17" s="130"/>
       <c r="J17" s="130"/>
       <c r="K17" s="130"/>
-      <c r="L17" s="132">
-        <f t="shared" si="0"/>
+      <c r="L17" s="130"/>
+      <c r="M17" s="132">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="126">
         <v>13</v>
       </c>
@@ -7076,19 +7097,25 @@
       <c r="C18" s="125" t="s">
         <v>201</v>
       </c>
-      <c r="D18" s="133"/>
-      <c r="F18" s="128"/>
-      <c r="G18" s="140"/>
-      <c r="H18" s="130"/>
+      <c r="D18" s="140">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="E18" s="133">
+        <v>35</v>
+      </c>
+      <c r="G18" s="128"/>
+      <c r="H18" s="140"/>
       <c r="I18" s="130"/>
       <c r="J18" s="130"/>
       <c r="K18" s="130"/>
-      <c r="L18" s="132">
-        <f t="shared" si="0"/>
+      <c r="L18" s="130"/>
+      <c r="M18" s="132">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="126">
         <v>14</v>
       </c>
@@ -7096,21 +7123,24 @@
         <v>1</v>
       </c>
       <c r="C19" s="125" t="s">
-        <v>204</v>
-      </c>
-      <c r="D19" s="133"/>
-      <c r="F19" s="128"/>
-      <c r="G19" s="140"/>
-      <c r="H19" s="130"/>
-      <c r="I19" s="130"/>
-      <c r="J19" s="130"/>
-      <c r="K19" s="130"/>
-      <c r="L19" s="132">
+        <v>195</v>
+      </c>
+      <c r="D19" s="140">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E19" s="133">
+        <v>4</v>
+      </c>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19" s="124"/>
+      <c r="J19" s="124"/>
+      <c r="K19" s="124"/>
+      <c r="L19" s="124"/>
+      <c r="M19" s="124"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="126">
         <v>15</v>
       </c>
@@ -7118,86 +7148,107 @@
         <v>1</v>
       </c>
       <c r="C20" s="125" t="s">
-        <v>198</v>
-      </c>
-      <c r="D20" s="133"/>
-      <c r="F20"/>
+        <v>200</v>
+      </c>
+      <c r="D20" s="140">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E20" s="133">
+        <v>4</v>
+      </c>
       <c r="G20"/>
-      <c r="H20" s="124"/>
+      <c r="H20"/>
       <c r="I20" s="124"/>
       <c r="J20" s="124"/>
       <c r="K20" s="124"/>
       <c r="L20" s="124"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="126">
-        <v>16</v>
-      </c>
-      <c r="B21" s="123" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="125" t="s">
-        <v>203</v>
-      </c>
-      <c r="D21" s="133"/>
-      <c r="F21"/>
+      <c r="M20" s="124"/>
+    </row>
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="154" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="155"/>
+      <c r="C21" s="156"/>
+      <c r="D21" s="131">
+        <f>SUM(D12:D20)</f>
+        <v>52.5</v>
+      </c>
+      <c r="E21" s="131">
+        <f>SUM(E12:E20)</f>
+        <v>105</v>
+      </c>
       <c r="G21"/>
-      <c r="H21" s="124"/>
+      <c r="H21"/>
       <c r="I21" s="124"/>
       <c r="J21" s="124"/>
       <c r="K21" s="124"/>
       <c r="L21" s="124"/>
-    </row>
-    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="152" t="s">
+      <c r="M21" s="124"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="126">
+        <v>16</v>
+      </c>
+      <c r="B22" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="153"/>
-      <c r="C22" s="154"/>
-      <c r="D22" s="131">
-        <f>SUM(D12:D21)</f>
-        <v>0</v>
-      </c>
-      <c r="F22"/>
+      <c r="C22" s="140" t="s">
+        <v>193</v>
+      </c>
+      <c r="D22" s="140">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E22" s="133">
+        <v>10</v>
+      </c>
       <c r="G22"/>
-      <c r="H22" s="124"/>
+      <c r="H22"/>
       <c r="I22" s="124"/>
       <c r="J22" s="124"/>
       <c r="K22" s="124"/>
       <c r="L22" s="124"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="124"/>
+    </row>
+    <row r="23" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="126">
         <v>17</v>
       </c>
       <c r="B23" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="140" t="s">
-        <v>195</v>
-      </c>
-      <c r="D23" s="133"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23" s="124"/>
-      <c r="I23" s="124"/>
-      <c r="J23" s="124"/>
-      <c r="K23" s="124"/>
-      <c r="L23" s="124"/>
-    </row>
-    <row r="24" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C23" s="141" t="s">
+        <v>257</v>
+      </c>
+      <c r="D23" s="140">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="E23" s="133">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="126">
         <v>18</v>
       </c>
       <c r="B24" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="141" t="s">
-        <v>196</v>
-      </c>
-      <c r="D24" s="133"/>
-    </row>
-    <row r="25" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C24" s="142" t="s">
+        <v>255</v>
+      </c>
+      <c r="D24" s="140">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E24" s="133">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="126">
         <v>19</v>
       </c>
@@ -7205,11 +7256,17 @@
         <v>2</v>
       </c>
       <c r="C25" s="142" t="s">
-        <v>190</v>
-      </c>
-      <c r="D25" s="133"/>
-    </row>
-    <row r="26" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+      <c r="D25" s="140">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E25" s="133">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="126">
         <v>20</v>
       </c>
@@ -7217,11 +7274,17 @@
         <v>2</v>
       </c>
       <c r="C26" s="142" t="s">
-        <v>233</v>
-      </c>
-      <c r="D26" s="133"/>
-    </row>
-    <row r="27" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+      <c r="D26" s="140">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="E26" s="133">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="126">
         <v>21</v>
       </c>
@@ -7229,348 +7292,284 @@
         <v>2</v>
       </c>
       <c r="C27" s="142" t="s">
-        <v>250</v>
-      </c>
-      <c r="D27" s="133"/>
-    </row>
-    <row r="28" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+      <c r="D27" s="140">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E27" s="133">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="126">
         <v>22</v>
       </c>
       <c r="B28" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="142" t="s">
-        <v>251</v>
-      </c>
-      <c r="D28" s="133"/>
-    </row>
-    <row r="29" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="126">
-        <v>23</v>
-      </c>
-      <c r="B29" s="123" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="141" t="s">
-        <v>208</v>
-      </c>
-      <c r="D29" s="133"/>
-    </row>
-    <row r="30" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C28" s="141"/>
+      <c r="D28" s="140">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E28" s="133"/>
+    </row>
+    <row r="29" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="126"/>
+      <c r="B29" s="123"/>
+      <c r="C29" s="142"/>
+      <c r="D29" s="140">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="133"/>
+    </row>
+    <row r="30" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="126">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B30" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="142" t="s">
-        <v>209</v>
-      </c>
-      <c r="D30" s="133"/>
-    </row>
-    <row r="31" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C30" s="125" t="s">
+        <v>195</v>
+      </c>
+      <c r="D30" s="140">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E30" s="133">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="126">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B31" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="142" t="s">
+      <c r="C31" s="125" t="s">
+        <v>200</v>
+      </c>
+      <c r="D31" s="140">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="E31" s="133">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="154" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="155"/>
+      <c r="C32" s="156"/>
+      <c r="D32" s="131">
+        <f>SUM(D22:D31)</f>
+        <v>120</v>
+      </c>
+      <c r="E32" s="131">
+        <f>SUM(E22:E31)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="126">
+        <v>36</v>
+      </c>
+      <c r="B33" s="123" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="140" t="s">
+        <v>193</v>
+      </c>
+      <c r="D33" s="140">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E33" s="133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="126">
+        <v>37</v>
+      </c>
+      <c r="B34" s="123" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="125" t="s">
+        <v>202</v>
+      </c>
+      <c r="D34" s="140">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="E34" s="133">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="126">
+        <v>38</v>
+      </c>
+      <c r="B35" s="123" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="125" t="s">
+        <v>203</v>
+      </c>
+      <c r="D35" s="140">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="E35" s="133">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="126">
+        <v>39</v>
+      </c>
+      <c r="B36" s="123" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="125" t="s">
+        <v>208</v>
+      </c>
+      <c r="D36" s="140">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E36" s="133">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="126">
+        <v>40</v>
+      </c>
+      <c r="B37" s="123" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="140" t="s">
+        <v>204</v>
+      </c>
+      <c r="D37" s="140">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E37" s="133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="126">
+        <v>41</v>
+      </c>
+      <c r="B38" s="123" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="140" t="s">
         <v>205</v>
       </c>
-      <c r="D31" s="133"/>
-    </row>
-    <row r="32" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="126">
-        <v>26</v>
-      </c>
-      <c r="B32" s="123" t="s">
+      <c r="D38" s="140">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E38" s="133">
         <v>2</v>
       </c>
-      <c r="C32" s="142" t="s">
+    </row>
+    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="126">
+        <v>42</v>
+      </c>
+      <c r="B39" s="123" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="140" t="s">
         <v>207</v>
       </c>
-      <c r="D32" s="133"/>
-    </row>
-    <row r="33" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="126">
-        <v>27</v>
-      </c>
-      <c r="B33" s="123" t="s">
+      <c r="D39" s="140">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E39" s="133">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="126">
+        <v>43</v>
+      </c>
+      <c r="B40" s="123" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="140" t="s">
+        <v>206</v>
+      </c>
+      <c r="D40" s="140">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E40" s="133">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="126">
+        <v>44</v>
+      </c>
+      <c r="B41" s="137" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="125" t="s">
+        <v>195</v>
+      </c>
+      <c r="D41" s="140">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E41" s="133">
         <v>2</v>
       </c>
-      <c r="C33" s="142" t="s">
-        <v>206</v>
-      </c>
-      <c r="D33" s="133"/>
-    </row>
-    <row r="34" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="126">
+    </row>
+    <row r="42" spans="1:5" ht="12" x14ac:dyDescent="0.2">
+      <c r="A42" s="154"/>
+      <c r="B42" s="155"/>
+      <c r="C42" s="156"/>
+      <c r="D42" s="131">
+        <f>SUM(D33:D41)</f>
         <v>28</v>
       </c>
-      <c r="B34" s="123" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" s="141" t="s">
-        <v>234</v>
-      </c>
-      <c r="D34" s="133"/>
-    </row>
-    <row r="35" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="126">
-        <v>29</v>
-      </c>
-      <c r="B35" s="123" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" s="142" t="s">
-        <v>235</v>
-      </c>
-      <c r="D35" s="133"/>
-    </row>
-    <row r="36" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="126">
-        <v>30</v>
-      </c>
-      <c r="B36" s="123" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="142" t="s">
-        <v>236</v>
-      </c>
-      <c r="D36" s="133"/>
-    </row>
-    <row r="37" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="126">
-        <v>31</v>
-      </c>
-      <c r="B37" s="123" t="s">
-        <v>2</v>
-      </c>
-      <c r="C37" s="142" t="s">
-        <v>237</v>
-      </c>
-      <c r="D37" s="133"/>
-    </row>
-    <row r="38" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="126">
-        <v>32</v>
-      </c>
-      <c r="B38" s="123" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" s="142" t="s">
-        <v>238</v>
-      </c>
-      <c r="D38" s="133"/>
-    </row>
-    <row r="39" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="126">
-        <v>33</v>
-      </c>
-      <c r="B39" s="123" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="141" t="s">
-        <v>239</v>
-      </c>
-      <c r="D39" s="133"/>
-    </row>
-    <row r="40" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="126"/>
-      <c r="B40" s="123"/>
-      <c r="C40" s="142"/>
-      <c r="D40" s="133"/>
-    </row>
-    <row r="41" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="126"/>
-      <c r="B41" s="123"/>
-      <c r="C41" s="142"/>
-      <c r="D41" s="133"/>
-    </row>
-    <row r="42" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="126"/>
-      <c r="B42" s="123"/>
-      <c r="C42" s="142"/>
-      <c r="D42" s="133"/>
-    </row>
-    <row r="43" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="126"/>
-      <c r="B43" s="123"/>
-      <c r="C43" s="142"/>
-      <c r="D43" s="133"/>
-    </row>
-    <row r="44" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="126">
-        <v>34</v>
-      </c>
-      <c r="B44" s="123" t="s">
-        <v>2</v>
-      </c>
-      <c r="C44" s="125" t="s">
-        <v>198</v>
-      </c>
-      <c r="D44" s="133"/>
-    </row>
-    <row r="45" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="126">
-        <v>35</v>
-      </c>
-      <c r="B45" s="123" t="s">
-        <v>2</v>
-      </c>
-      <c r="C45" s="125" t="s">
-        <v>203</v>
-      </c>
-      <c r="D45" s="133"/>
-    </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="152" t="s">
-        <v>3</v>
-      </c>
-      <c r="B46" s="153"/>
-      <c r="C46" s="154"/>
-      <c r="D46" s="131">
-        <f>SUM(D23:D45)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="126">
-        <v>36</v>
-      </c>
-      <c r="B47" s="123" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" s="140" t="s">
-        <v>195</v>
-      </c>
-      <c r="D47" s="133"/>
-    </row>
-    <row r="48" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="126">
-        <v>37</v>
-      </c>
-      <c r="B48" s="123" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="125" t="s">
-        <v>210</v>
-      </c>
-      <c r="D48" s="133"/>
-    </row>
-    <row r="49" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="126">
-        <v>38</v>
-      </c>
-      <c r="B49" s="123" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" s="125" t="s">
-        <v>211</v>
-      </c>
-      <c r="D49" s="133"/>
-    </row>
-    <row r="50" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="126">
-        <v>39</v>
-      </c>
-      <c r="B50" s="123" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" s="125" t="s">
-        <v>216</v>
-      </c>
-      <c r="D50" s="133"/>
-    </row>
-    <row r="51" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="126">
-        <v>40</v>
-      </c>
-      <c r="B51" s="123" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" s="140" t="s">
-        <v>212</v>
-      </c>
-      <c r="D51" s="133"/>
-    </row>
-    <row r="52" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="126">
-        <v>41</v>
-      </c>
-      <c r="B52" s="123" t="s">
-        <v>3</v>
-      </c>
-      <c r="C52" s="140" t="s">
-        <v>213</v>
-      </c>
-      <c r="D52" s="133"/>
-    </row>
-    <row r="53" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="126">
-        <v>42</v>
-      </c>
-      <c r="B53" s="123" t="s">
-        <v>3</v>
-      </c>
-      <c r="C53" s="140" t="s">
-        <v>215</v>
-      </c>
-      <c r="D53" s="133"/>
-    </row>
-    <row r="54" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="126">
-        <v>43</v>
-      </c>
-      <c r="B54" s="123" t="s">
-        <v>3</v>
-      </c>
-      <c r="C54" s="140" t="s">
-        <v>214</v>
-      </c>
-      <c r="D54" s="133"/>
-    </row>
-    <row r="55" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="126">
-        <v>44</v>
-      </c>
-      <c r="B55" s="137" t="s">
-        <v>3</v>
-      </c>
-      <c r="C55" s="125" t="s">
-        <v>198</v>
-      </c>
-      <c r="D55" s="133"/>
-    </row>
-    <row r="56" spans="1:4" ht="12" x14ac:dyDescent="0.2">
-      <c r="A56" s="152"/>
-      <c r="B56" s="153"/>
-      <c r="C56" s="154"/>
-      <c r="D56" s="131">
-        <f>SUM(D47:D55)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="D57" s="143">
-        <f>SUM(D11,D22,D46,D56)</f>
-        <v>62</v>
+      <c r="E42" s="131">
+        <f>SUM(E33:E41)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="E43" s="143">
+        <f>SUM(E11,E21,E32,E42)</f>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="G1:M1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="G2:M2"/>
+    <mergeCell ref="I3:M3"/>
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
     <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7587,7 +7586,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7598,27 +7597,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="164" t="s">
+      <c r="A1" s="166" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="164"/>
-      <c r="C1" s="164"/>
+      <c r="B1" s="166"/>
+      <c r="C1" s="166"/>
     </row>
     <row r="2" spans="1:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="167" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="165"/>
-      <c r="C3" s="165"/>
+      <c r="B3" s="167"/>
+      <c r="C3" s="167"/>
     </row>
     <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="B4" s="147">
-        <f>'Backlog Produto'!$D$57</f>
-        <v>62</v>
+        <f>'Backlog Produto'!$E$43</f>
+        <v>418</v>
       </c>
       <c r="C4" s="27" t="s">
         <v>13</v>
@@ -7629,27 +7628,27 @@
         <v>188</v>
       </c>
       <c r="B5" s="26">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="C5" s="56" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="B6" s="15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6" s="29"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="B7" s="15">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>13</v>
@@ -7657,11 +7656,11 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="B8" s="145">
         <f>B6*B7*2</f>
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C8" s="29" t="s">
         <v>13</v>
@@ -7669,23 +7668,23 @@
     </row>
     <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="B9" s="144">
         <f>B11/2</f>
-        <v>3.1</v>
+        <v>7.5109374999999998</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="56" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="B10" s="146">
         <f>B4+(B4*B5)</f>
-        <v>62</v>
+        <v>480.7</v>
       </c>
       <c r="C10" s="56" t="s">
         <v>13</v>
@@ -7693,11 +7692,11 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="B11" s="145">
         <f>B10/B8*2</f>
-        <v>6.2</v>
+        <v>15.021875</v>
       </c>
       <c r="C11" s="29" t="s">
         <v>28</v>
@@ -7705,29 +7704,29 @@
     </row>
     <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="B12" s="144">
         <f>B11/4</f>
-        <v>1.55</v>
+        <v>3.7554687499999999</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="165" t="s">
+      <c r="A14" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="165"/>
-      <c r="C14" s="165"/>
+      <c r="B14" s="167"/>
+      <c r="C14" s="167"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="149">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C15" s="2"/>
     </row>
@@ -7735,10 +7734,7 @@
       <c r="A16" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="5">
-        <f>B10*B15</f>
-        <v>1240</v>
-      </c>
+      <c r="B16" s="5"/>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -7762,11 +7758,11 @@
     </row>
     <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="B19" s="148">
         <f>B16+B18</f>
-        <v>1240</v>
+        <v>0</v>
       </c>
       <c r="C19" s="2"/>
     </row>
@@ -7775,7 +7771,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="26">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="C20" s="2"/>
     </row>
@@ -7785,17 +7781,17 @@
       </c>
       <c r="B21" s="7">
         <f>B19*B20</f>
-        <v>248</v>
+        <v>0</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="B22" s="148">
         <f>B19+B21</f>
-        <v>1488</v>
+        <v>0</v>
       </c>
       <c r="C22" s="2"/>
     </row>
@@ -7819,7 +7815,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -7836,62 +7832,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="168" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="167"/>
-      <c r="J1" s="167"/>
-      <c r="K1" s="167"/>
+      <c r="B1" s="169"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="169"/>
+      <c r="H1" s="169"/>
+      <c r="I1" s="169"/>
+      <c r="J1" s="169"/>
+      <c r="K1" s="169"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="169" t="s">
+      <c r="A2" s="171" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="171"/>
+      <c r="B2" s="173"/>
       <c r="C2" s="82" t="e">
         <f>Planejamento!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D2" s="168" t="s">
+      <c r="D2" s="170" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="168"/>
+      <c r="E2" s="170"/>
       <c r="F2" s="83" t="e">
         <f>Planejamento!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="G2" s="169" t="s">
+      <c r="G2" s="171" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="171"/>
+      <c r="H2" s="172"/>
+      <c r="I2" s="172"/>
+      <c r="J2" s="173"/>
       <c r="K2" s="82">
         <f>Planejamento!$B$10</f>
-        <v>62</v>
+        <v>480.7</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="84"/>
       <c r="B3" s="85"/>
-      <c r="C3" s="172" t="s">
+      <c r="C3" s="174" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="172"/>
-      <c r="E3" s="172"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
       <c r="F3" s="86"/>
-      <c r="G3" s="173" t="s">
+      <c r="G3" s="175" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="174"/>
-      <c r="I3" s="175"/>
+      <c r="H3" s="176"/>
+      <c r="I3" s="177"/>
       <c r="J3" s="87"/>
       <c r="K3" s="88"/>
     </row>
@@ -7935,7 +7931,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="92" t="s">
-        <v>274</v>
+        <v>0</v>
       </c>
       <c r="C5" s="93">
         <v>45168</v>
@@ -7947,16 +7943,16 @@
         <v>18</v>
       </c>
       <c r="F5" s="95" t="s">
-        <v>275</v>
+        <v>249</v>
       </c>
       <c r="G5" s="93">
         <v>45168</v>
       </c>
-      <c r="H5" s="93" t="s">
-        <v>276</v>
+      <c r="H5" s="93">
+        <v>45182</v>
       </c>
       <c r="I5" s="94" t="s">
-        <v>276</v>
+        <v>250</v>
       </c>
       <c r="J5" s="96" t="e">
         <f>E5-I5</f>
@@ -7970,8 +7966,12 @@
       <c r="A6" s="91">
         <v>2</v>
       </c>
-      <c r="B6" s="92"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="92" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="93">
+        <v>45182</v>
+      </c>
       <c r="D6" s="93"/>
       <c r="E6" s="98"/>
       <c r="F6" s="95"/>
@@ -7985,7 +7985,9 @@
       <c r="A7" s="91">
         <v>3</v>
       </c>
-      <c r="B7" s="92"/>
+      <c r="B7" s="92" t="s">
+        <v>2</v>
+      </c>
       <c r="C7" s="93"/>
       <c r="D7" s="93"/>
       <c r="E7" s="98"/>
@@ -8000,9 +8002,13 @@
       <c r="A8" s="91">
         <v>4</v>
       </c>
-      <c r="B8" s="92"/>
+      <c r="B8" s="92" t="s">
+        <v>3</v>
+      </c>
       <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
+      <c r="D8" s="93">
+        <v>45259</v>
+      </c>
       <c r="E8" s="98"/>
       <c r="F8" s="95"/>
       <c r="G8" s="93"/>
@@ -8128,25 +8134,33 @@
     <mergeCell ref="G3:I3"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F14">
-    <cfRule type="expression" dxfId="13" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="21" stopIfTrue="1">
       <formula>$F5="Planned"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="22" stopIfTrue="1">
       <formula>$F5="Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="23" stopIfTrue="1" operator="equal">
       <formula>"Unplanned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:D14">
-    <cfRule type="expression" dxfId="10" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="24" stopIfTrue="1">
       <formula>OR($F5="Planned",$F5="Unplanned")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="25" stopIfTrue="1">
       <formula>$F5="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:H14 H5">
+  <conditionalFormatting sqref="G6:H14">
+    <cfRule type="expression" dxfId="10" priority="5" stopIfTrue="1">
+      <formula>OR($F6="Planned",$F6="Unplanned")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="6" stopIfTrue="1">
+      <formula>$F6="Ongoing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
     <cfRule type="expression" dxfId="8" priority="3" stopIfTrue="1">
       <formula>OR($F5="Planned",$F5="Unplanned")</formula>
     </cfRule>
@@ -8154,11 +8168,11 @@
       <formula>$F5="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="H5">
+    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
       <formula>OR($F5="Planned",$F5="Unplanned")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
       <formula>$F5="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8174,18 +8188,18 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+      <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="58" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" style="58" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" style="58" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="58" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" style="58" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" style="58" bestFit="1" customWidth="1"/>
@@ -8193,7 +8207,7 @@
     <col min="7" max="7" width="9.85546875" style="58" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="13.140625" style="58" customWidth="1"/>
     <col min="10" max="10" width="26" style="58" customWidth="1"/>
-    <col min="11" max="11" width="30" style="58" customWidth="1"/>
+    <col min="11" max="11" width="48.5703125" style="58" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="58"/>
     <col min="13" max="14" width="22" style="58" customWidth="1"/>
     <col min="15" max="256" width="9.140625" style="58"/>
@@ -9019,19 +9033,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="57" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="168" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="167"/>
-      <c r="J1" s="167"/>
-      <c r="K1" s="167"/>
+      <c r="B1" s="169"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="169"/>
+      <c r="H1" s="169"/>
+      <c r="I1" s="169"/>
+      <c r="J1" s="169"/>
+      <c r="K1" s="169"/>
     </row>
     <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
@@ -9208,10 +9222,10 @@
       <c r="A33" s="65"/>
       <c r="B33" s="65"/>
       <c r="C33" s="65"/>
-      <c r="D33" s="176" t="s">
+      <c r="D33" s="183" t="s">
         <v>110</v>
       </c>
-      <c r="E33" s="177"/>
+      <c r="E33" s="184"/>
       <c r="F33" s="65"/>
       <c r="G33" s="65"/>
       <c r="H33" s="65"/>
@@ -9323,137 +9337,137 @@
     </row>
     <row r="40" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:11" s="57" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="184" t="s">
+      <c r="A41" s="190" t="s">
         <v>117</v>
       </c>
-      <c r="B41" s="184"/>
-      <c r="C41" s="184"/>
-      <c r="D41" s="184"/>
-      <c r="E41" s="184"/>
-      <c r="F41" s="184"/>
-      <c r="G41" s="184"/>
-      <c r="H41" s="184"/>
-      <c r="I41" s="184"/>
-      <c r="J41" s="184"/>
-      <c r="K41" s="184"/>
+      <c r="B41" s="190"/>
+      <c r="C41" s="190"/>
+      <c r="D41" s="190"/>
+      <c r="E41" s="190"/>
+      <c r="F41" s="190"/>
+      <c r="G41" s="190"/>
+      <c r="H41" s="190"/>
+      <c r="I41" s="190"/>
+      <c r="J41" s="190"/>
+      <c r="K41" s="190"/>
     </row>
     <row r="42" spans="1:11" s="57" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="185" t="s">
+      <c r="A42" s="191" t="s">
         <v>118</v>
       </c>
-      <c r="B42" s="185"/>
-      <c r="C42" s="185"/>
-      <c r="D42" s="185"/>
-      <c r="E42" s="185"/>
-      <c r="F42" s="185"/>
-      <c r="G42" s="185"/>
-      <c r="H42" s="185"/>
-      <c r="I42" s="185"/>
-      <c r="J42" s="185"/>
-      <c r="K42" s="185"/>
+      <c r="B42" s="191"/>
+      <c r="C42" s="191"/>
+      <c r="D42" s="191"/>
+      <c r="E42" s="191"/>
+      <c r="F42" s="191"/>
+      <c r="G42" s="191"/>
+      <c r="H42" s="191"/>
+      <c r="I42" s="191"/>
+      <c r="J42" s="191"/>
+      <c r="K42" s="191"/>
     </row>
     <row r="43" spans="1:11" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="186" t="s">
+      <c r="A43" s="192" t="s">
         <v>132</v>
       </c>
-      <c r="B43" s="186"/>
-      <c r="C43" s="186"/>
-      <c r="D43" s="186"/>
-      <c r="E43" s="186"/>
-      <c r="F43" s="186"/>
-      <c r="G43" s="186"/>
-      <c r="H43" s="186"/>
-      <c r="I43" s="186"/>
-      <c r="J43" s="186"/>
-      <c r="K43" s="186"/>
+      <c r="B43" s="192"/>
+      <c r="C43" s="192"/>
+      <c r="D43" s="192"/>
+      <c r="E43" s="192"/>
+      <c r="F43" s="192"/>
+      <c r="G43" s="192"/>
+      <c r="H43" s="192"/>
+      <c r="I43" s="192"/>
+      <c r="J43" s="192"/>
+      <c r="K43" s="192"/>
     </row>
     <row r="44" spans="1:11" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="187" t="s">
+      <c r="A44" s="193" t="s">
         <v>119</v>
       </c>
-      <c r="B44" s="187"/>
-      <c r="C44" s="187"/>
-      <c r="D44" s="187"/>
-      <c r="E44" s="187"/>
-      <c r="F44" s="187"/>
-      <c r="G44" s="187"/>
-      <c r="H44" s="187"/>
-      <c r="I44" s="187"/>
-      <c r="J44" s="187"/>
-      <c r="K44" s="187"/>
+      <c r="B44" s="193"/>
+      <c r="C44" s="193"/>
+      <c r="D44" s="193"/>
+      <c r="E44" s="193"/>
+      <c r="F44" s="193"/>
+      <c r="G44" s="193"/>
+      <c r="H44" s="193"/>
+      <c r="I44" s="193"/>
+      <c r="J44" s="193"/>
+      <c r="K44" s="193"/>
     </row>
     <row r="45" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="178" t="s">
+      <c r="A46" s="185" t="s">
         <v>120</v>
       </c>
-      <c r="B46" s="179"/>
-      <c r="C46" s="179"/>
-      <c r="D46" s="179"/>
-      <c r="E46" s="179"/>
-      <c r="F46" s="179"/>
-      <c r="G46" s="179"/>
-      <c r="H46" s="179"/>
-      <c r="I46" s="179"/>
-      <c r="J46" s="179"/>
-      <c r="K46" s="179"/>
+      <c r="B46" s="186"/>
+      <c r="C46" s="186"/>
+      <c r="D46" s="186"/>
+      <c r="E46" s="186"/>
+      <c r="F46" s="186"/>
+      <c r="G46" s="186"/>
+      <c r="H46" s="186"/>
+      <c r="I46" s="186"/>
+      <c r="J46" s="186"/>
+      <c r="K46" s="186"/>
     </row>
     <row r="47" spans="1:11" s="71" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="81" t="s">
         <v>121</v>
       </c>
       <c r="B47" s="80"/>
-      <c r="C47" s="180" t="s">
+      <c r="C47" s="187" t="s">
         <v>122</v>
       </c>
-      <c r="D47" s="180"/>
-      <c r="E47" s="180"/>
-      <c r="F47" s="180"/>
-      <c r="G47" s="180"/>
-      <c r="H47" s="180"/>
-      <c r="I47" s="180"/>
-      <c r="J47" s="180"/>
-      <c r="K47" s="180"/>
+      <c r="D47" s="187"/>
+      <c r="E47" s="187"/>
+      <c r="F47" s="187"/>
+      <c r="G47" s="187"/>
+      <c r="H47" s="187"/>
+      <c r="I47" s="187"/>
+      <c r="J47" s="187"/>
+      <c r="K47" s="187"/>
     </row>
     <row r="48" spans="1:11" s="72" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="183"/>
-      <c r="B48" s="183" t="s">
+      <c r="A48" s="180"/>
+      <c r="B48" s="180" t="s">
         <v>131</v>
       </c>
-      <c r="C48" s="183" t="s">
+      <c r="C48" s="180" t="s">
         <v>123</v>
       </c>
-      <c r="D48" s="183" t="s">
+      <c r="D48" s="180" t="s">
         <v>124</v>
       </c>
-      <c r="E48" s="183" t="s">
+      <c r="E48" s="180" t="s">
         <v>95</v>
       </c>
-      <c r="F48" s="183" t="s">
+      <c r="F48" s="180" t="s">
         <v>125</v>
       </c>
-      <c r="G48" s="183" t="s">
+      <c r="G48" s="180" t="s">
         <v>99</v>
       </c>
-      <c r="H48" s="190" t="s">
+      <c r="H48" s="181" t="s">
         <v>126</v>
       </c>
-      <c r="I48" s="191"/>
-      <c r="J48" s="191"/>
-      <c r="K48" s="191"/>
+      <c r="I48" s="182"/>
+      <c r="J48" s="182"/>
+      <c r="K48" s="182"/>
     </row>
     <row r="49" spans="1:11" s="72" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="183"/>
-      <c r="B49" s="183"/>
-      <c r="C49" s="183"/>
-      <c r="D49" s="183"/>
-      <c r="E49" s="183"/>
-      <c r="F49" s="183"/>
-      <c r="G49" s="183"/>
-      <c r="H49" s="181" t="s">
+      <c r="A49" s="180"/>
+      <c r="B49" s="180"/>
+      <c r="C49" s="180"/>
+      <c r="D49" s="180"/>
+      <c r="E49" s="180"/>
+      <c r="F49" s="180"/>
+      <c r="G49" s="180"/>
+      <c r="H49" s="188" t="s">
         <v>127</v>
       </c>
-      <c r="I49" s="182"/>
+      <c r="I49" s="189"/>
       <c r="J49" s="73" t="s">
         <v>128</v>
       </c>
@@ -9484,8 +9498,8 @@
       <c r="G50" s="75" t="s">
         <v>100</v>
       </c>
-      <c r="H50" s="188"/>
-      <c r="I50" s="189"/>
+      <c r="H50" s="178"/>
+      <c r="I50" s="179"/>
       <c r="J50" s="79"/>
       <c r="K50" s="79" t="s">
         <v>134</v>
@@ -9495,19 +9509,31 @@
       <c r="A51" s="100">
         <v>2</v>
       </c>
-      <c r="B51" s="101"/>
-      <c r="C51" s="74"/>
-      <c r="D51" s="75"/>
-      <c r="E51" s="75"/>
-      <c r="F51" s="76" t="e">
+      <c r="B51" s="101" t="s">
+        <v>252</v>
+      </c>
+      <c r="C51" s="74">
+        <v>45175</v>
+      </c>
+      <c r="D51" s="75" t="s">
+        <v>93</v>
+      </c>
+      <c r="E51" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="F51" s="76" t="str">
         <f t="shared" ref="F51:F58" si="0">IF(OR((CODE($D51)*CODE($E51))=$D$36,(CODE($D51)*CODE($E51))=$D$35),$D$15,IF(OR((CODE($D51)*CODE($E51))=$D$34,(CODE($D51)*CODE($E51))=$D$37),$D$16,IF(OR((CODE($D51)*CODE($E51))=$D$38,(CODE($D51)*CODE($E51))=$D$39),$D$17,)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G51" s="75"/>
+        <v>Alta</v>
+      </c>
+      <c r="G51" s="75" t="s">
+        <v>100</v>
+      </c>
       <c r="H51" s="77"/>
       <c r="I51" s="78"/>
       <c r="J51" s="79"/>
-      <c r="K51" s="79"/>
+      <c r="K51" s="79" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="52" spans="1:11" s="72" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="100">
@@ -9648,8 +9674,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="G59" s="75"/>
-      <c r="H59" s="188"/>
-      <c r="I59" s="189"/>
+      <c r="H59" s="178"/>
+      <c r="I59" s="179"/>
       <c r="J59" s="79"/>
       <c r="K59" s="79"/>
     </row>
@@ -9666,22 +9692,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="G60" s="75"/>
-      <c r="H60" s="188"/>
-      <c r="I60" s="189"/>
+      <c r="H60" s="178"/>
+      <c r="I60" s="179"/>
       <c r="J60" s="79"/>
       <c r="K60" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="H48:K48"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="A46:K46"/>
@@ -9693,15 +9710,24 @@
     <mergeCell ref="A42:K42"/>
     <mergeCell ref="A43:K43"/>
     <mergeCell ref="A44:K44"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="H48:K48"/>
   </mergeCells>
   <conditionalFormatting sqref="F50:F60">
-    <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
       <formula>$D$15</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="equal">
       <formula>$D$16</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
       <formula>$D$17</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9733,7 +9759,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -9746,33 +9772,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="192" t="s">
-        <v>255</v>
-      </c>
-      <c r="B1" s="193"/>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
+      <c r="A1" s="194" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
     </row>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="84"/>
       <c r="B2" s="85"/>
-      <c r="C2" s="172" t="s">
+      <c r="C2" s="174" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="172"/>
+      <c r="D2" s="174"/>
     </row>
     <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="89" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="D3" s="89" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -9780,52 +9806,34 @@
         <v>1</v>
       </c>
       <c r="B4" s="92" t="s">
-        <v>269</v>
-      </c>
-      <c r="C4" s="93">
-        <v>45168</v>
-      </c>
-      <c r="D4" s="75" t="s">
-        <v>268</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="C4" s="93"/>
+      <c r="D4" s="75"/>
     </row>
     <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="91">
         <v>2</v>
       </c>
-      <c r="B5" s="92" t="s">
-        <v>270</v>
-      </c>
-      <c r="C5" s="93">
-        <v>45175</v>
-      </c>
+      <c r="B5" s="92"/>
+      <c r="C5" s="93"/>
       <c r="D5" s="75"/>
     </row>
     <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="91">
         <v>3</v>
       </c>
-      <c r="B6" s="92" t="s">
-        <v>271</v>
-      </c>
-      <c r="C6" s="93">
-        <v>45175</v>
-      </c>
+      <c r="B6" s="92"/>
+      <c r="C6" s="93"/>
       <c r="D6" s="75"/>
     </row>
     <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="91">
         <v>4</v>
       </c>
-      <c r="B7" s="92" t="s">
-        <v>272</v>
-      </c>
-      <c r="C7" s="93">
-        <v>45182</v>
-      </c>
-      <c r="D7" s="75" t="s">
-        <v>268</v>
-      </c>
+      <c r="B7" s="92"/>
+      <c r="C7" s="93"/>
+      <c r="D7" s="75"/>
     </row>
     <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="91">
@@ -9891,10 +9899,10 @@
     <mergeCell ref="C2:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:C13">
-    <cfRule type="expression" dxfId="3" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="22" stopIfTrue="1">
       <formula>OR(#REF!="Planned",#REF!="Unplanned")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="23" stopIfTrue="1">
       <formula>#REF!="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9969,7 +9977,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="122" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -9985,7 +9993,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="122" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
@@ -10001,7 +10009,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="122" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -10017,7 +10025,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="122" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -10033,7 +10041,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="122" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
@@ -10049,7 +10057,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="122" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -10322,7 +10330,7 @@
       </c>
       <c r="B16" s="45">
         <f>Planejamento!B8</f>
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C16" s="45" t="s">
         <v>12</v>
@@ -10374,116 +10382,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="57" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="202" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="200"/>
-      <c r="I1" s="200"/>
-      <c r="J1" s="200"/>
-      <c r="K1" s="200"/>
-      <c r="L1" s="200"/>
-      <c r="M1" s="200"/>
-      <c r="N1" s="200"/>
+      <c r="B1" s="202"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="202"/>
+      <c r="E1" s="202"/>
+      <c r="F1" s="202"/>
+      <c r="G1" s="202"/>
+      <c r="H1" s="202"/>
+      <c r="I1" s="202"/>
+      <c r="J1" s="202"/>
+      <c r="K1" s="202"/>
+      <c r="L1" s="202"/>
+      <c r="M1" s="202"/>
+      <c r="N1" s="202"/>
     </row>
     <row r="2" spans="1:23" s="103" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="201" t="s">
+      <c r="A2" s="203" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="201"/>
-      <c r="C2" s="201"/>
-      <c r="D2" s="201"/>
-      <c r="E2" s="201"/>
-      <c r="F2" s="201"/>
-      <c r="G2" s="201"/>
-      <c r="H2" s="201"/>
-      <c r="I2" s="201"/>
-      <c r="J2" s="201"/>
-      <c r="K2" s="201"/>
-      <c r="L2" s="201"/>
-      <c r="M2" s="201"/>
-      <c r="N2" s="201"/>
+      <c r="B2" s="203"/>
+      <c r="C2" s="203"/>
+      <c r="D2" s="203"/>
+      <c r="E2" s="203"/>
+      <c r="F2" s="203"/>
+      <c r="G2" s="203"/>
+      <c r="H2" s="203"/>
+      <c r="I2" s="203"/>
+      <c r="J2" s="203"/>
+      <c r="K2" s="203"/>
+      <c r="L2" s="203"/>
+      <c r="M2" s="203"/>
+      <c r="N2" s="203"/>
     </row>
     <row r="3" spans="1:23" s="103" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="202" t="s">
+      <c r="A3" s="204" t="s">
         <v>169</v>
       </c>
-      <c r="B3" s="202"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="202"/>
-      <c r="F3" s="202"/>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="202"/>
-      <c r="J3" s="202"/>
-      <c r="K3" s="202"/>
-      <c r="L3" s="202"/>
-      <c r="M3" s="202"/>
-      <c r="N3" s="202"/>
+      <c r="B3" s="204"/>
+      <c r="C3" s="204"/>
+      <c r="D3" s="204"/>
+      <c r="E3" s="204"/>
+      <c r="F3" s="204"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="204"/>
+      <c r="J3" s="204"/>
+      <c r="K3" s="204"/>
+      <c r="L3" s="204"/>
+      <c r="M3" s="204"/>
+      <c r="N3" s="204"/>
     </row>
     <row r="4" spans="1:23" s="103" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="203" t="s">
+      <c r="A4" s="205" t="s">
         <v>136</v>
       </c>
-      <c r="B4" s="203"/>
-      <c r="C4" s="203"/>
-      <c r="D4" s="203"/>
-      <c r="E4" s="203"/>
-      <c r="F4" s="203"/>
-      <c r="G4" s="203"/>
-      <c r="H4" s="203"/>
-      <c r="I4" s="203"/>
-      <c r="J4" s="203"/>
-      <c r="K4" s="203"/>
-      <c r="L4" s="203"/>
-      <c r="M4" s="203"/>
-      <c r="N4" s="203"/>
+      <c r="B4" s="205"/>
+      <c r="C4" s="205"/>
+      <c r="D4" s="205"/>
+      <c r="E4" s="205"/>
+      <c r="F4" s="205"/>
+      <c r="G4" s="205"/>
+      <c r="H4" s="205"/>
+      <c r="I4" s="205"/>
+      <c r="J4" s="205"/>
+      <c r="K4" s="205"/>
+      <c r="L4" s="205"/>
+      <c r="M4" s="205"/>
+      <c r="N4" s="205"/>
     </row>
     <row r="5" spans="1:23" s="103" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="204" t="s">
+      <c r="A5" s="206" t="s">
         <v>170</v>
       </c>
-      <c r="B5" s="204"/>
-      <c r="C5" s="204"/>
-      <c r="D5" s="204"/>
-      <c r="E5" s="204"/>
-      <c r="F5" s="204"/>
-      <c r="G5" s="204"/>
-      <c r="H5" s="204"/>
-      <c r="I5" s="204"/>
-      <c r="J5" s="204"/>
-      <c r="K5" s="204"/>
-      <c r="L5" s="204"/>
-      <c r="M5" s="204"/>
-      <c r="N5" s="204"/>
+      <c r="B5" s="206"/>
+      <c r="C5" s="206"/>
+      <c r="D5" s="206"/>
+      <c r="E5" s="206"/>
+      <c r="F5" s="206"/>
+      <c r="G5" s="206"/>
+      <c r="H5" s="206"/>
+      <c r="I5" s="206"/>
+      <c r="J5" s="206"/>
+      <c r="K5" s="206"/>
+      <c r="L5" s="206"/>
+      <c r="M5" s="206"/>
+      <c r="N5" s="206"/>
     </row>
     <row r="6" spans="1:23" s="22" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:23" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A7" s="198" t="s">
+      <c r="A7" s="200" t="s">
         <v>153</v>
       </c>
-      <c r="B7" s="199"/>
-      <c r="D7" s="198" t="s">
+      <c r="B7" s="201"/>
+      <c r="D7" s="200" t="s">
         <v>171</v>
       </c>
-      <c r="E7" s="199"/>
-      <c r="G7" s="194" t="s">
+      <c r="E7" s="201"/>
+      <c r="G7" s="196" t="s">
         <v>138</v>
       </c>
-      <c r="H7" s="194"/>
-      <c r="I7" s="194"/>
-      <c r="J7" s="194"/>
-      <c r="K7" s="194"/>
-      <c r="M7" s="198" t="s">
+      <c r="H7" s="196"/>
+      <c r="I7" s="196"/>
+      <c r="J7" s="196"/>
+      <c r="K7" s="196"/>
+      <c r="M7" s="200" t="s">
         <v>172</v>
       </c>
-      <c r="N7" s="199"/>
+      <c r="N7" s="201"/>
     </row>
     <row r="8" spans="1:23" s="22" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="104" t="s">
@@ -10583,13 +10591,13 @@
       <c r="B11" s="106"/>
       <c r="D11" s="102"/>
       <c r="E11" s="106"/>
-      <c r="G11" s="194" t="s">
+      <c r="G11" s="196" t="s">
         <v>143</v>
       </c>
-      <c r="H11" s="194"/>
-      <c r="I11" s="194"/>
-      <c r="J11" s="194"/>
-      <c r="K11" s="194"/>
+      <c r="H11" s="196"/>
+      <c r="I11" s="196"/>
+      <c r="J11" s="196"/>
+      <c r="K11" s="196"/>
       <c r="M11" s="108" t="s">
         <v>158</v>
       </c>
@@ -10692,12 +10700,12 @@
       <c r="B16" s="106"/>
       <c r="D16" s="102"/>
       <c r="E16" s="106"/>
-      <c r="G16" s="195" t="s">
+      <c r="G16" s="197" t="s">
         <v>147</v>
       </c>
-      <c r="H16" s="196"/>
-      <c r="I16" s="196"/>
-      <c r="J16" s="197"/>
+      <c r="H16" s="198"/>
+      <c r="I16" s="198"/>
+      <c r="J16" s="199"/>
       <c r="K16" s="107">
         <f>SUM(K9,K10,K13,K14,K15)</f>
         <v>14</v>
@@ -10862,42 +10870,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="202" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="200"/>
-      <c r="I1" s="200"/>
-      <c r="J1" s="200"/>
-      <c r="K1" s="200"/>
-      <c r="L1" s="200"/>
-      <c r="M1" s="200"/>
-      <c r="N1" s="200"/>
+      <c r="B1" s="202"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="202"/>
+      <c r="E1" s="202"/>
+      <c r="F1" s="202"/>
+      <c r="G1" s="202"/>
+      <c r="H1" s="202"/>
+      <c r="I1" s="202"/>
+      <c r="J1" s="202"/>
+      <c r="K1" s="202"/>
+      <c r="L1" s="202"/>
+      <c r="M1" s="202"/>
+      <c r="N1" s="202"/>
     </row>
     <row r="2" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="206" t="s">
+      <c r="A3" s="208" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="206"/>
-      <c r="C3" s="206"/>
-      <c r="E3" s="193" t="s">
+      <c r="B3" s="208"/>
+      <c r="C3" s="208"/>
+      <c r="E3" s="195" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="193"/>
-      <c r="G3" s="193"/>
-      <c r="H3" s="193"/>
-      <c r="I3" s="193"/>
-      <c r="J3" s="193"/>
-      <c r="K3" s="193"/>
-      <c r="L3" s="193"/>
-      <c r="M3" s="193"/>
-      <c r="N3" s="193"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="195"/>
+      <c r="I3" s="195"/>
+      <c r="J3" s="195"/>
+      <c r="K3" s="195"/>
+      <c r="L3" s="195"/>
+      <c r="M3" s="195"/>
+      <c r="N3" s="195"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -10910,25 +10918,25 @@
       <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="207" t="s">
+      <c r="E4" s="209" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="205" t="s">
+      <c r="F4" s="207" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="205"/>
-      <c r="H4" s="205" t="s">
+      <c r="G4" s="207"/>
+      <c r="H4" s="207" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="205"/>
-      <c r="J4" s="205" t="s">
+      <c r="I4" s="207"/>
+      <c r="J4" s="207" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="205"/>
-      <c r="L4" s="205" t="s">
+      <c r="K4" s="207"/>
+      <c r="L4" s="207" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="205"/>
+      <c r="M4" s="207"/>
       <c r="N4" s="120"/>
     </row>
     <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
@@ -10941,23 +10949,23 @@
       <c r="C5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="207"/>
-      <c r="F5" s="205" t="s">
+      <c r="E5" s="209"/>
+      <c r="F5" s="207" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="205"/>
-      <c r="H5" s="205" t="s">
+      <c r="G5" s="207"/>
+      <c r="H5" s="207" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="205"/>
-      <c r="J5" s="205" t="s">
+      <c r="I5" s="207"/>
+      <c r="J5" s="207" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="205"/>
-      <c r="L5" s="205" t="s">
+      <c r="K5" s="207"/>
+      <c r="L5" s="207" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="205"/>
+      <c r="M5" s="207"/>
       <c r="N5" s="27" t="s">
         <v>184</v>
       </c>
@@ -10973,7 +10981,7 @@
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="207"/>
+      <c r="E6" s="209"/>
       <c r="F6" s="116">
         <f>B6*G6</f>
         <v>8.6450000000000014</v>
@@ -11405,11 +11413,11 @@
       <c r="N15" s="53"/>
     </row>
     <row r="16" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="206" t="s">
+      <c r="A16" s="208" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="206"/>
-      <c r="C16" s="206"/>
+      <c r="B16" s="208"/>
+      <c r="C16" s="208"/>
       <c r="E16" s="27" t="s">
         <v>185</v>
       </c>

</xml_diff>